<commit_message>
removed some un needed files, ran the program from scratch over night and changed some things as a result. Most notably the larger bounds of C hindered the algorithm so returned to old bounds. Updated README.md
</commit_message>
<xml_diff>
--- a/stored_variables/6/spectrum/solid_angle_of_binwidth_1.5.xlsx
+++ b/stored_variables/6/spectrum/solid_angle_of_binwidth_1.5.xlsx
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>3.555034517827098e-05</v>
+        <v>3.593675756095905e-05</v>
       </c>
     </row>
     <row r="54">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.0001499193678815009</v>
+        <v>0.0001515435597034</v>
       </c>
     </row>
     <row r="55">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.0002133220950620968</v>
+        <v>0.000215623132953908</v>
       </c>
     </row>
     <row r="56">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.00026090740429838</v>
+        <v>0.0002637092816778138</v>
       </c>
     </row>
     <row r="57">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.0003003366366068642</v>
+        <v>0.0003035476017859354</v>
       </c>
     </row>
     <row r="58">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.0003345519471363904</v>
+        <v>0.0003381127472178012</v>
       </c>
     </row>
     <row r="59">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.000365157959248138</v>
+        <v>0.0003690271544326033</v>
       </c>
     </row>
     <row r="60">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.0003927054479244963</v>
+        <v>0.000396847905260332</v>
       </c>
     </row>
     <row r="61">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.0004116131243156612</v>
+        <v>0.0004159344571100114</v>
       </c>
     </row>
     <row r="62">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.0004215287194826389</v>
+        <v>0.0004259319785643563</v>
       </c>
     </row>
     <row r="63">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.0004329680204201878</v>
+        <v>0.0004374675536883943</v>
       </c>
     </row>
     <row r="64">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.0004335140795217773</v>
+        <v>0.0004379939085233069</v>
       </c>
     </row>
     <row r="65">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.0004306793118091697</v>
+        <v>0.0004351040850615983</v>
       </c>
     </row>
     <row r="66">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.000430853602792051</v>
+        <v>0.0004352540265304451</v>
       </c>
     </row>
     <row r="67">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.0004275620960688068</v>
+        <v>0.0004319035614071445</v>
       </c>
     </row>
     <row r="68">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.0004277913218706684</v>
+        <v>0.0004321092625899597</v>
       </c>
     </row>
     <row r="69">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.0004250055009073985</v>
+        <v>0.0004292702006612846</v>
       </c>
     </row>
     <row r="70">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.0004228448033719743</v>
+        <v>0.0004270627392766278</v>
       </c>
     </row>
     <row r="71">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.0004239279148187512</v>
+        <v>0.0004281312409821128</v>
       </c>
     </row>
     <row r="72">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.0004207065028135159</v>
+        <v>0.0004248532044143352</v>
       </c>
     </row>
     <row r="73">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.0004188950000898414</v>
+        <v>0.0004229991311774837</v>
       </c>
     </row>
     <row r="74">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.0004177879262982798</v>
+        <v>0.0004218567235136354</v>
       </c>
     </row>
     <row r="75">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.0004161541087997072</v>
+        <v>0.0004201825633336685</v>
       </c>
     </row>
     <row r="76">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.000414530203184065</v>
+        <v>0.0004185186951316869</v>
       </c>
     </row>
     <row r="77">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.00041364697668031</v>
+        <v>0.000417602846426938</v>
       </c>
     </row>
     <row r="78">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.0004122715502239909</v>
+        <v>0.0004161902504205417</v>
       </c>
     </row>
     <row r="79">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.0004108221637588265</v>
+        <v>0.0004147031830243576</v>
       </c>
     </row>
     <row r="80">
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.0004096829801745913</v>
+        <v>0.000413529580102239</v>
       </c>
     </row>
     <row r="81">
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.0004083048003969928</v>
+        <v>0.0004121148160164887</v>
       </c>
     </row>
     <row r="82">
@@ -1252,7 +1252,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.000406862118840806</v>
+        <v>0.0004106352524865064</v>
       </c>
     </row>
     <row r="83">
@@ -1262,7 +1262,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.0004048897381441954</v>
+        <v>0.0004086213975886232</v>
       </c>
     </row>
     <row r="84">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.0004028548152650907</v>
+        <v>0.0004065447986042101</v>
       </c>
     </row>
     <row r="85">
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.0004030313785021564</v>
+        <v>0.0004066997520940158</v>
       </c>
     </row>
     <row r="86">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.0004009353356239542</v>
+        <v>0.000404561867845346</v>
       </c>
     </row>
     <row r="87">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.0003990574727024446</v>
+        <v>0.0004026444501043212</v>
       </c>
     </row>
     <row r="88">
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.0003989363648061247</v>
+        <v>0.0004024994859207084</v>
       </c>
     </row>
     <row r="89">
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.0003958758416526175</v>
+        <v>0.0003993894477975947</v>
       </c>
     </row>
     <row r="90">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.0003963481472224831</v>
+        <v>0.0003998434797629707</v>
       </c>
     </row>
     <row r="91">
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.0003935660043131057</v>
+        <v>0.0003970148289060268</v>
       </c>
     </row>
     <row r="92">
@@ -1352,7 +1352,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.0003926047213294587</v>
+        <v>0.00039602313501778</v>
       </c>
     </row>
     <row r="93">
@@ -1362,7 +1362,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.0003921957194867911</v>
+        <v>0.0003955885175455898</v>
       </c>
     </row>
     <row r="94">
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.0003896978154273117</v>
+        <v>0.0003930474581551607</v>
       </c>
     </row>
     <row r="95">
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0.0003879778872852383</v>
+        <v>0.0003912912731991943</v>
       </c>
     </row>
     <row r="96">
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0.0003888913034387522</v>
+        <v>0.0003921906210066474</v>
       </c>
     </row>
     <row r="97">
@@ -1402,7 +1402,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0.0003864555027531076</v>
+        <v>0.0003897129494025698</v>
       </c>
     </row>
     <row r="98">
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>0.0003847385807851588</v>
+        <v>0.0003879603815032482</v>
       </c>
     </row>
     <row r="99">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.0003833101632207365</v>
+        <v>0.0003864989618147206</v>
       </c>
     </row>
     <row r="100">
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.0003823798889419178</v>
+        <v>0.0003855400139545792</v>
       </c>
     </row>
     <row r="101">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.0003808959832217021</v>
+        <v>0.0003840230107555525</v>
       </c>
     </row>
     <row r="102">
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.0003800231846962505</v>
+        <v>0.0003831223211301325</v>
       </c>
     </row>
     <row r="103">
@@ -1462,7 +1462,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.0003787985053964116</v>
+        <v>0.0003818670570629477</v>
       </c>
     </row>
     <row r="104">
@@ -1472,7 +1472,7 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.0003775220355609999</v>
+        <v>0.0003805597613561832</v>
       </c>
     </row>
     <row r="105">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.0003763123164691662</v>
+        <v>0.0003793199021878973</v>
       </c>
     </row>
     <row r="106">
@@ -1492,7 +1492,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.0003753834721291029</v>
+        <v>0.0003783634321298716</v>
       </c>
     </row>
     <row r="107">
@@ -1502,7 +1502,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.0003738582884169851</v>
+        <v>0.0003768059932755624</v>
       </c>
     </row>
     <row r="108">
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.0003723090465390228</v>
+        <v>0.0003752246726803825</v>
       </c>
     </row>
     <row r="109">
@@ -1522,7 +1522,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.0003703147663915771</v>
+        <v>0.0003731950899226947</v>
       </c>
     </row>
     <row r="110">
@@ -1532,7 +1532,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.0003708564450509586</v>
+        <v>0.0003737209491395047</v>
       </c>
     </row>
     <row r="111">
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.0003692936849598854</v>
+        <v>0.0003721264995354606</v>
       </c>
     </row>
     <row r="112">
@@ -1552,7 +1552,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.0003661394555223999</v>
+        <v>0.0003689289855517769</v>
       </c>
     </row>
     <row r="113">
@@ -1562,7 +1562,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.0003677518034462862</v>
+        <v>0.0003705337746653547</v>
       </c>
     </row>
     <row r="114">
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0.0003655619830654415</v>
+        <v>0.000368308146199389</v>
       </c>
     </row>
     <row r="115">
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0.0003633477249052533</v>
+        <v>0.0003660583624327277</v>
       </c>
     </row>
     <row r="116">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.0003639338802955942</v>
+        <v>0.0003666295382234343</v>
       </c>
     </row>
     <row r="117">
@@ -1602,7 +1602,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.000360905380881177</v>
+        <v>0.0003635599997078612</v>
       </c>
     </row>
     <row r="118">
@@ -1612,7 +1612,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.0003616496134403292</v>
+        <v>0.0003642905375492919</v>
       </c>
     </row>
     <row r="119">
@@ -1622,7 +1622,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>0.0003589836612440921</v>
+        <v>0.0003615866754717689</v>
       </c>
     </row>
     <row r="120">
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.0003586545057971932</v>
+        <v>0.0003612363468075908</v>
       </c>
     </row>
     <row r="121">
@@ -1642,7 +1642,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.0003572851390436271</v>
+        <v>0.0003598386851055284</v>
       </c>
     </row>
     <row r="122">
@@ -1652,7 +1652,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>0.0003552627682178307</v>
+        <v>0.0003577837046819631</v>
       </c>
     </row>
     <row r="123">
@@ -1662,7 +1662,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>0.000355991253391125</v>
+        <v>0.0003584987252789081</v>
       </c>
     </row>
     <row r="124">
@@ -1672,7 +1672,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>0.0003538425509580239</v>
+        <v>0.0003563168534016945</v>
       </c>
     </row>
     <row r="125">
@@ -1682,7 +1682,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>0.0003523064775552182</v>
+        <v>0.000354752088054082</v>
       </c>
     </row>
     <row r="126">
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>0.0003510023458465823</v>
+        <v>0.0003534210769387413</v>
       </c>
     </row>
     <row r="127">
@@ -1702,7 +1702,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>0.000351577716628466</v>
+        <v>0.0003539821548427104</v>
       </c>
     </row>
     <row r="128">
@@ -1712,7 +1712,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>0.0003497329965062418</v>
+        <v>0.0003521072118726592</v>
       </c>
     </row>
     <row r="129">
@@ -1722,7 +1722,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>0.0003482727480078143</v>
+        <v>0.0003506194530396858</v>
       </c>
     </row>
     <row r="130">
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>0.0003471918457130495</v>
+        <v>0.0003495137343678371</v>
       </c>
     </row>
     <row r="131">
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0.0003459166682323688</v>
+        <v>0.0003482126104791015</v>
       </c>
     </row>
     <row r="132">
@@ -1752,7 +1752,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.0003450121385296304</v>
+        <v>0.000347284786022647</v>
       </c>
     </row>
     <row r="133">
@@ -1762,7 +1762,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0.0003441551153798489</v>
+        <v>0.0003464048631298515</v>
       </c>
     </row>
     <row r="134">
@@ -1772,7 +1772,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>0.0003428898081830248</v>
+        <v>0.0003451141399111081</v>
       </c>
     </row>
     <row r="135">
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>0.0003420037419458396</v>
+        <v>0.0003442052369033101</v>
       </c>
     </row>
     <row r="136">
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>0.0003409642512561341</v>
+        <v>0.0003431421163657902</v>
       </c>
     </row>
     <row r="137">
@@ -1802,7 +1802,7 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.0003401116478779383</v>
+        <v>0.0003422672114553374</v>
       </c>
     </row>
     <row r="138">
@@ -1812,7 +1812,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>0.0003388736746101154</v>
+        <v>0.0003410046435388376</v>
       </c>
     </row>
     <row r="139">
@@ -1822,7 +1822,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>0.0003375314524092948</v>
+        <v>0.0003396373767297795</v>
       </c>
     </row>
     <row r="140">
@@ -1832,7 +1832,7 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>0.0003358886963546153</v>
+        <v>0.0003379679938512654</v>
       </c>
     </row>
     <row r="141">
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.0003354084060029757</v>
+        <v>0.0003374682581436203</v>
       </c>
     </row>
     <row r="142">
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>0.000335339947436519</v>
+        <v>0.0003373828211740152</v>
       </c>
     </row>
     <row r="143">
@@ -1862,7 +1862,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>0.0003341227017620662</v>
+        <v>0.0003361418940335148</v>
       </c>
     </row>
     <row r="144">
@@ -1872,7 +1872,7 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>0.00033207749758594</v>
+        <v>0.0003340683104139937</v>
       </c>
     </row>
     <row r="145">
@@ -1882,7 +1882,7 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>0.0003312903579159858</v>
+        <v>0.0003332603792787691</v>
       </c>
     </row>
     <row r="146">
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>0.0003313050527899743</v>
+        <v>0.000333258964412428</v>
       </c>
     </row>
     <row r="147">
@@ -1902,7 +1902,7 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>0.0003292615909204</v>
+        <v>0.000331187771404419</v>
       </c>
     </row>
     <row r="148">
@@ -1912,7 +1912,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>0.0003285586686839772</v>
+        <v>0.0003304649063622755</v>
       </c>
     </row>
     <row r="149">
@@ -1922,7 +1922,7 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>0.0003281557099455048</v>
+        <v>0.0003300437026302535</v>
       </c>
     </row>
     <row r="150">
@@ -1932,7 +1932,7 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>0.0003257012589268539</v>
+        <v>0.0003275598667318103</v>
       </c>
     </row>
     <row r="151">
@@ -1942,7 +1942,7 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>0.0003267548797591513</v>
+        <v>0.0003286035701261121</v>
       </c>
     </row>
     <row r="152">
@@ -1952,7 +1952,7 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>0.0003232494516713991</v>
+        <v>0.0003250632641991225</v>
       </c>
     </row>
     <row r="153">
@@ -1962,7 +1962,7 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>0.0003250040009110892</v>
+        <v>0.0003268118716776178</v>
       </c>
     </row>
     <row r="154">
@@ -1972,7 +1972,7 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>0.0003216036761652816</v>
+        <v>0.0003233777753795233</v>
       </c>
     </row>
     <row r="155">
@@ -1982,7 +1982,7 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>0.0003229925476805688</v>
+        <v>0.000324758703692006</v>
       </c>
     </row>
     <row r="156">
@@ -1992,7 +1992,7 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>0.0003201418145303214</v>
+        <v>0.0003218776204052817</v>
       </c>
     </row>
     <row r="157">
@@ -2002,7 +2002,7 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>0.000320248644150286</v>
+        <v>0.0003219698183388626</v>
       </c>
     </row>
     <row r="158">
@@ -2012,7 +2012,7 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>0.0003190223168449742</v>
+        <v>0.0003207219515500583</v>
       </c>
     </row>
     <row r="159">
@@ -2022,7 +2022,7 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>0.0003170908140849527</v>
+        <v>0.0003187655976118252</v>
       </c>
     </row>
     <row r="160">
@@ -2032,7 +2032,7 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>0.0003180001649884715</v>
+        <v>0.0003196646469918138</v>
       </c>
     </row>
     <row r="161">
@@ -2042,7 +2042,7 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>0.0003162397687041758</v>
+        <v>0.0003178804770795185</v>
       </c>
     </row>
     <row r="162">
@@ -2052,7 +2052,7 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>0.0003145769095121084</v>
+        <v>0.0003161945118360113</v>
       </c>
     </row>
     <row r="163">
@@ -2062,7 +2062,7 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>0.0003134432120734631</v>
+        <v>0.0003150406306689916</v>
       </c>
     </row>
     <row r="164">
@@ -2072,7 +2072,7 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>0.0003146575408718508</v>
+        <v>0.0003162461659292052</v>
       </c>
     </row>
     <row r="165">
@@ -2082,7 +2082,7 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>0.0003125469589903859</v>
+        <v>0.0003141108539967413</v>
       </c>
     </row>
     <row r="166">
@@ -2092,7 +2092,7 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>0.0003112855176085909</v>
+        <v>0.0003128288940002364</v>
       </c>
     </row>
     <row r="167">
@@ -2102,7 +2102,7 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>0.0003100280302651524</v>
+        <v>0.0003115510265504111</v>
       </c>
     </row>
     <row r="168">
@@ -2112,7 +2112,7 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>0.0003092511280115309</v>
+        <v>0.0003107562641389259</v>
       </c>
     </row>
     <row r="169">
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>0.0003083299370878324</v>
+        <v>0.0003098165764499503</v>
       </c>
     </row>
     <row r="170">
@@ -2132,7 +2132,7 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>0.0003092240795977303</v>
+        <v>0.0003107006744555037</v>
       </c>
     </row>
     <row r="171">
@@ -2142,7 +2142,7 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.0003073409132646066</v>
+        <v>0.0003087948373032586</v>
       </c>
     </row>
     <row r="172">
@@ -2152,7 +2152,7 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0.000306190334101746</v>
+        <v>0.0003076249911566795</v>
       </c>
     </row>
     <row r="173">
@@ -2162,7 +2162,7 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>0.0003052301583171102</v>
+        <v>0.000306646592275246</v>
       </c>
     </row>
     <row r="174">
@@ -2172,7 +2172,7 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>0.0003044380934618369</v>
+        <v>0.0003058372234231701</v>
       </c>
     </row>
     <row r="175">
@@ -2182,7 +2182,7 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>0.0003034966340186114</v>
+        <v>0.0003048778751969262</v>
       </c>
     </row>
     <row r="176">
@@ -2192,7 +2192,7 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>0.0003026259806206762</v>
+        <v>0.0003039897626878081</v>
       </c>
     </row>
     <row r="177">
@@ -2202,7 +2202,7 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>0.0003015325041571299</v>
+        <v>0.0003028779396616262</v>
       </c>
     </row>
     <row r="178">
@@ -2212,7 +2212,7 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>0.0003004752131084703</v>
+        <v>0.0003018027089918605</v>
       </c>
     </row>
     <row r="179">
@@ -2222,7 +2222,7 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>0.0002990230263434832</v>
+        <v>0.0003003309756282361</v>
       </c>
     </row>
     <row r="180">
@@ -2232,7 +2232,7 @@
         </is>
       </c>
       <c r="B180" t="n">
-        <v>0.0002995223870199927</v>
+        <v>0.0003008190703272518</v>
       </c>
     </row>
     <row r="181">
@@ -2242,7 +2242,7 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>0.0002988108367780307</v>
+        <v>0.0003000912702239552</v>
       </c>
     </row>
     <row r="182">
@@ -2252,7 +2252,7 @@
         </is>
       </c>
       <c r="B182" t="n">
-        <v>0.0002979445170234493</v>
+        <v>0.0002992081922949427</v>
       </c>
     </row>
     <row r="183">
@@ -2262,7 +2262,7 @@
         </is>
       </c>
       <c r="B183" t="n">
-        <v>0.000296910950500212</v>
+        <v>0.0002981572023800001</v>
       </c>
     </row>
     <row r="184">
@@ -2272,7 +2272,7 @@
         </is>
       </c>
       <c r="B184" t="n">
-        <v>0.0002956647197199176</v>
+        <v>0.0002968929016218871</v>
       </c>
     </row>
     <row r="185">
@@ -2282,7 +2282,7 @@
         </is>
       </c>
       <c r="B185" t="n">
-        <v>0.00029336376564416</v>
+        <v>0.0002945698681346833</v>
       </c>
     </row>
     <row r="186">
@@ -2292,7 +2292,7 @@
         </is>
       </c>
       <c r="B186" t="n">
-        <v>0.0002950745229729085</v>
+        <v>0.0002962745053306618</v>
       </c>
     </row>
     <row r="187">
@@ -2302,7 +2302,7 @@
         </is>
       </c>
       <c r="B187" t="n">
-        <v>0.0002938737749548913</v>
+        <v>0.0002950561604348952</v>
       </c>
     </row>
     <row r="188">
@@ -2312,7 +2312,7 @@
         </is>
       </c>
       <c r="B188" t="n">
-        <v>0.0002924430500218594</v>
+        <v>0.0002936071187599449</v>
       </c>
     </row>
     <row r="189">
@@ -2322,7 +2322,7 @@
         </is>
       </c>
       <c r="B189" t="n">
-        <v>0.0002904541541479048</v>
+        <v>0.0002915979970389563</v>
       </c>
     </row>
     <row r="190">
@@ -2332,7 +2332,7 @@
         </is>
       </c>
       <c r="B190" t="n">
-        <v>0.0002918619557108622</v>
+        <v>0.0002929984710721533</v>
       </c>
     </row>
     <row r="191">
@@ -2342,7 +2342,7 @@
         </is>
       </c>
       <c r="B191" t="n">
-        <v>0.0002901446899059311</v>
+        <v>0.0002912621954351671</v>
       </c>
     </row>
     <row r="192">
@@ -2352,7 +2352,7 @@
         </is>
       </c>
       <c r="B192" t="n">
-        <v>0.0002880941995683955</v>
+        <v>0.000289191717096851</v>
       </c>
     </row>
     <row r="193">
@@ -2362,7 +2362,7 @@
         </is>
       </c>
       <c r="B193" t="n">
-        <v>0.0002895016476157399</v>
+        <v>0.0002905918345945429</v>
       </c>
     </row>
     <row r="194">
@@ -2372,7 +2372,7 @@
         </is>
       </c>
       <c r="B194" t="n">
-        <v>0.000287136751306585</v>
+        <v>0.0002882061102246386</v>
       </c>
     </row>
     <row r="195">
@@ -2382,7 +2382,7 @@
         </is>
       </c>
       <c r="B195" t="n">
-        <v>0.0002869057626804734</v>
+        <v>0.0002879619368493403</v>
       </c>
     </row>
     <row r="196">
@@ -2392,7 +2392,7 @@
         </is>
       </c>
       <c r="B196" t="n">
-        <v>0.0002864097524060458</v>
+        <v>0.000287451950889823</v>
       </c>
     </row>
     <row r="197">
@@ -2402,7 +2402,7 @@
         </is>
       </c>
       <c r="B197" t="n">
-        <v>0.0002845681705323521</v>
+        <v>0.0002855918865287804</v>
       </c>
     </row>
     <row r="198">
@@ -2412,7 +2412,7 @@
         </is>
       </c>
       <c r="B198" t="n">
-        <v>0.0002850424471409127</v>
+        <v>0.0002860555605451279</v>
       </c>
     </row>
     <row r="199">
@@ -2422,7 +2422,7 @@
         </is>
       </c>
       <c r="B199" t="n">
-        <v>0.0002825337273175309</v>
+        <v>0.0002835264204764304</v>
       </c>
     </row>
     <row r="200">
@@ -2432,7 +2432,7 @@
         </is>
       </c>
       <c r="B200" t="n">
-        <v>0.0002841311204872118</v>
+        <v>0.0002851172048486924</v>
       </c>
     </row>
     <row r="201">
@@ -2442,7 +2442,7 @@
         </is>
       </c>
       <c r="B201" t="n">
-        <v>0.0002811432108466458</v>
+        <v>0.0002821075075577386</v>
       </c>
     </row>
     <row r="202">
@@ -2452,7 +2452,7 @@
         </is>
       </c>
       <c r="B202" t="n">
-        <v>0.0002819109032094206</v>
+        <v>0.0002828657937414204</v>
       </c>
     </row>
     <row r="203">
@@ -2462,7 +2462,7 @@
         </is>
       </c>
       <c r="B203" t="n">
-        <v>0.0002802022777033897</v>
+        <v>0.0002811399652224901</v>
       </c>
     </row>
     <row r="204">
@@ -2472,7 +2472,7 @@
         </is>
       </c>
       <c r="B204" t="n">
-        <v>0.000279412918078285</v>
+        <v>0.0002803363954949141</v>
       </c>
     </row>
     <row r="205">
@@ -2482,7 +2482,7 @@
         </is>
       </c>
       <c r="B205" t="n">
-        <v>0.000279638285034772</v>
+        <v>0.0002805507804472175</v>
       </c>
     </row>
     <row r="206">
@@ -2492,7 +2492,7 @@
         </is>
       </c>
       <c r="B206" t="n">
-        <v>0.000277137345219741</v>
+        <v>0.0002780305717861402</v>
       </c>
     </row>
     <row r="207">
@@ -2502,7 +2502,7 @@
         </is>
       </c>
       <c r="B207" t="n">
-        <v>0.0002783095856305217</v>
+        <v>0.0002791947551727923</v>
       </c>
     </row>
     <row r="208">
@@ -2512,7 +2512,7 @@
         </is>
       </c>
       <c r="B208" t="n">
-        <v>0.000276682367333657</v>
+        <v>0.0002775512924659566</v>
       </c>
     </row>
     <row r="209">
@@ -2522,7 +2522,7 @@
         </is>
       </c>
       <c r="B209" t="n">
-        <v>0.0002750195660529691</v>
+        <v>0.0002758721424938408</v>
       </c>
     </row>
     <row r="210">
@@ -2532,7 +2532,7 @@
         </is>
       </c>
       <c r="B210" t="n">
-        <v>0.0002763339343645773</v>
+        <v>0.0002771789713221269</v>
       </c>
     </row>
     <row r="211">
@@ -2542,7 +2542,7 @@
         </is>
       </c>
       <c r="B211" t="n">
-        <v>0.0002741788219101251</v>
+        <v>0.0002750063093707718</v>
       </c>
     </row>
     <row r="212">
@@ -2552,7 +2552,7 @@
         </is>
       </c>
       <c r="B212" t="n">
-        <v>0.0002730344840862734</v>
+        <v>0.0002738475880196725</v>
       </c>
     </row>
     <row r="213">
@@ -2562,7 +2562,7 @@
         </is>
       </c>
       <c r="B213" t="n">
-        <v>0.0002723542785263976</v>
+        <v>0.0002731543361841542</v>
       </c>
     </row>
     <row r="214">
@@ -2572,7 +2572,7 @@
         </is>
       </c>
       <c r="B214" t="n">
-        <v>0.0002736674281395212</v>
+        <v>0.0002744599206318294</v>
       </c>
     </row>
     <row r="215">
@@ -2582,7 +2582,7 @@
         </is>
       </c>
       <c r="B215" t="n">
-        <v>0.0002714925005118159</v>
+        <v>0.0002722680561773755</v>
       </c>
     </row>
     <row r="216">
@@ -2592,7 +2592,7 @@
         </is>
       </c>
       <c r="B216" t="n">
-        <v>0.0002701961824367481</v>
+        <v>0.0002709572416460071</v>
       </c>
     </row>
     <row r="217">
@@ -2602,7 +2602,7 @@
         </is>
       </c>
       <c r="B217" t="n">
-        <v>0.0002692990280900652</v>
+        <v>0.0002700468680473492</v>
       </c>
     </row>
     <row r="218">
@@ -2612,7 +2612,7 @@
         </is>
       </c>
       <c r="B218" t="n">
-        <v>0.0002699678735829995</v>
+        <v>0.0002707065422050371</v>
       </c>
     </row>
     <row r="219">
@@ -2622,7 +2622,7 @@
         </is>
       </c>
       <c r="B219" t="n">
-        <v>0.0002693477296818954</v>
+        <v>0.0002700739746291816</v>
       </c>
     </row>
     <row r="220">
@@ -2632,7 +2632,7 @@
         </is>
       </c>
       <c r="B220" t="n">
-        <v>0.0002679363152906458</v>
+        <v>0.000268648209722164</v>
       </c>
     </row>
     <row r="221">
@@ -2642,7 +2642,7 @@
         </is>
       </c>
       <c r="B221" t="n">
-        <v>0.0002669361144911567</v>
+        <v>0.0002676347800606617</v>
       </c>
     </row>
     <row r="222">
@@ -2652,7 +2652,7 @@
         </is>
       </c>
       <c r="B222" t="n">
-        <v>0.0002661605572463497</v>
+        <v>0.0002668467059146333</v>
       </c>
     </row>
     <row r="223">
@@ -2662,7 +2662,7 @@
         </is>
       </c>
       <c r="B223" t="n">
-        <v>0.0002655048769423081</v>
+        <v>0.0002661789475628069</v>
       </c>
     </row>
     <row r="224">
@@ -2672,7 +2672,7 @@
         </is>
       </c>
       <c r="B224" t="n">
-        <v>0.000264479776077026</v>
+        <v>0.0002651407917613514</v>
       </c>
     </row>
     <row r="225">
@@ -2682,7 +2682,7 @@
         </is>
       </c>
       <c r="B225" t="n">
-        <v>0.0002643780406711487</v>
+        <v>0.0002650285137764773</v>
       </c>
     </row>
     <row r="226">
@@ -2692,7 +2692,7 @@
         </is>
       </c>
       <c r="B226" t="n">
-        <v>0.0002633465411959344</v>
+        <v>0.0002639841465713411</v>
       </c>
     </row>
     <row r="227">
@@ -2702,7 +2702,7 @@
         </is>
       </c>
       <c r="B227" t="n">
-        <v>0.0002626407922091063</v>
+        <v>0.0002632664499342829</v>
       </c>
     </row>
     <row r="228">
@@ -2712,7 +2712,7 @@
         </is>
       </c>
       <c r="B228" t="n">
-        <v>0.0002622600880400986</v>
+        <v>0.0002628746566908114</v>
       </c>
     </row>
     <row r="229">
@@ -2722,7 +2722,7 @@
         </is>
       </c>
       <c r="B229" t="n">
-        <v>0.0002615789200375058</v>
+        <v>0.0002621817050365632</v>
       </c>
     </row>
     <row r="230">
@@ -2732,7 +2732,7 @@
         </is>
       </c>
       <c r="B230" t="n">
-        <v>0.0002606652395747953</v>
+        <v>0.0002612558180684492</v>
       </c>
     </row>
     <row r="231">
@@ -2742,7 +2742,7 @@
         </is>
       </c>
       <c r="B231" t="n">
-        <v>0.0002606111331787854</v>
+        <v>0.0002611915432647875</v>
       </c>
     </row>
     <row r="232">
@@ -2752,7 +2752,7 @@
         </is>
       </c>
       <c r="B232" t="n">
-        <v>0.0002597436055525871</v>
+        <v>0.0002603120733901953</v>
       </c>
     </row>
     <row r="233">
@@ -2762,7 +2762,7 @@
         </is>
       </c>
       <c r="B233" t="n">
-        <v>0.0002588024976685713</v>
+        <v>0.0002593589174863913</v>
       </c>
     </row>
     <row r="234">
@@ -2772,7 +2772,7 @@
         </is>
       </c>
       <c r="B234" t="n">
-        <v>0.0002583868702365483</v>
+        <v>0.0002589325345615546</v>
       </c>
     </row>
     <row r="235">
@@ -2782,7 +2782,7 @@
         </is>
       </c>
       <c r="B235" t="n">
-        <v>0.0002577191373887847</v>
+        <v>0.0002582535188955857</v>
       </c>
     </row>
     <row r="236">
@@ -2792,7 +2792,7 @@
         </is>
       </c>
       <c r="B236" t="n">
-        <v>0.0002569229836999657</v>
+        <v>0.0002574459153598252</v>
       </c>
     </row>
     <row r="237">
@@ -2802,7 +2802,7 @@
         </is>
       </c>
       <c r="B237" t="n">
-        <v>0.0002561230071916882</v>
+        <v>0.0002566345714019048</v>
       </c>
     </row>
     <row r="238">
@@ -2812,7 +2812,7 @@
         </is>
       </c>
       <c r="B238" t="n">
-        <v>0.0002555944219733048</v>
+        <v>0.0002560953412580119</v>
       </c>
     </row>
     <row r="239">
@@ -2822,7 +2822,7 @@
         </is>
       </c>
       <c r="B239" t="n">
-        <v>0.0002541225007953312</v>
+        <v>0.0002546110181071307</v>
       </c>
     </row>
     <row r="240">
@@ -2832,7 +2832,7 @@
         </is>
       </c>
       <c r="B240" t="n">
-        <v>0.0002531399422385797</v>
+        <v>0.0002536170623003083</v>
       </c>
     </row>
     <row r="241">
@@ -2842,7 +2842,7 @@
         </is>
       </c>
       <c r="B241" t="n">
-        <v>0.0002540913935639494</v>
+        <v>0.0002545604869998285</v>
       </c>
     </row>
     <row r="242">
@@ -2852,7 +2852,7 @@
         </is>
       </c>
       <c r="B242" t="n">
-        <v>0.0002535846740649857</v>
+        <v>0.0002540433885812472</v>
       </c>
     </row>
     <row r="243">
@@ -2862,7 +2862,7 @@
         </is>
       </c>
       <c r="B243" t="n">
-        <v>0.0002523661613704507</v>
+        <v>0.0002528132231102684</v>
       </c>
     </row>
     <row r="244">
@@ -2872,7 +2872,7 @@
         </is>
       </c>
       <c r="B244" t="n">
-        <v>0.0002510625005826549</v>
+        <v>0.0002514979970601795</v>
       </c>
     </row>
     <row r="245">
@@ -2882,7 +2882,7 @@
         </is>
       </c>
       <c r="B245" t="n">
-        <v>0.0002498342208707026</v>
+        <v>0.000250258397623348</v>
       </c>
     </row>
     <row r="246">
@@ -2892,7 +2892,7 @@
         </is>
       </c>
       <c r="B246" t="n">
-        <v>0.0002508929093859626</v>
+        <v>0.0002513092166064981</v>
       </c>
     </row>
     <row r="247">
@@ -2902,7 +2902,7 @@
         </is>
       </c>
       <c r="B247" t="n">
-        <v>0.0002501185422437492</v>
+        <v>0.0002505244316549598</v>
       </c>
     </row>
     <row r="248">
@@ -2912,7 +2912,7 @@
         </is>
       </c>
       <c r="B248" t="n">
-        <v>0.0002479284083395415</v>
+        <v>0.0002483217978108453</v>
       </c>
     </row>
     <row r="249">
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="B249" t="n">
-        <v>0.0002483516511736241</v>
+        <v>0.0002487364496337234</v>
       </c>
     </row>
     <row r="250">
@@ -2932,7 +2932,7 @@
         </is>
       </c>
       <c r="B250" t="n">
-        <v>0.0002486223339880509</v>
+        <v>0.0002489982405704849</v>
       </c>
     </row>
     <row r="251">
@@ -2942,7 +2942,7 @@
         </is>
       </c>
       <c r="B251" t="n">
-        <v>0.0002463580142724181</v>
+        <v>0.000246721587592677</v>
       </c>
     </row>
     <row r="252">
@@ -2952,7 +2952,7 @@
         </is>
       </c>
       <c r="B252" t="n">
-        <v>0.0002457557713428007</v>
+        <v>0.0002461096207777739</v>
       </c>
     </row>
     <row r="253">
@@ -2962,7 +2962,7 @@
         </is>
       </c>
       <c r="B253" t="n">
-        <v>0.0002465742943893912</v>
+        <v>0.0002469200427586266</v>
       </c>
     </row>
     <row r="254">
@@ -2972,7 +2972,7 @@
         </is>
       </c>
       <c r="B254" t="n">
-        <v>0.0002443944248818092</v>
+        <v>0.0002447284875204108</v>
       </c>
     </row>
     <row r="255">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="B255" t="n">
-        <v>0.0002446304314730218</v>
+        <v>0.000244955844029935</v>
       </c>
     </row>
     <row r="256">
@@ -2992,7 +2992,7 @@
         </is>
       </c>
       <c r="B256" t="n">
-        <v>0.0002445342029450458</v>
+        <v>0.0002448504953451124</v>
       </c>
     </row>
     <row r="257">
@@ -3002,7 +3002,7 @@
         </is>
       </c>
       <c r="B257" t="n">
-        <v>0.0002417728229871699</v>
+        <v>0.000242077213193348</v>
       </c>
     </row>
     <row r="258">
@@ -3012,7 +3012,7 @@
         </is>
       </c>
       <c r="B258" t="n">
-        <v>0.0002440160021892708</v>
+        <v>0.0002443139641313816</v>
       </c>
     </row>
     <row r="259">
@@ -3022,7 +3022,7 @@
         </is>
       </c>
       <c r="B259" t="n">
-        <v>0.0002409407384407077</v>
+        <v>0.0002412267040852207</v>
       </c>
     </row>
     <row r="260">
@@ -3032,7 +3032,7 @@
         </is>
       </c>
       <c r="B260" t="n">
-        <v>0.0002424747188935938</v>
+        <v>0.0002427535050651397</v>
       </c>
     </row>
     <row r="261">
@@ -3042,7 +3042,7 @@
         </is>
       </c>
       <c r="B261" t="n">
-        <v>0.0002405082107233358</v>
+        <v>0.0002407761643433032</v>
       </c>
     </row>
     <row r="262">
@@ -3052,7 +3052,7 @@
         </is>
       </c>
       <c r="B262" t="n">
-        <v>0.0002402804171041913</v>
+        <v>0.0002405397006748915</v>
       </c>
     </row>
     <row r="263">
@@ -3062,7 +3062,7 @@
         </is>
       </c>
       <c r="B263" t="n">
-        <v>0.0002398181757014241</v>
+        <v>0.0002400682776219764</v>
       </c>
     </row>
     <row r="264">
@@ -3072,7 +3072,7 @@
         </is>
       </c>
       <c r="B264" t="n">
-        <v>0.0002385852090798405</v>
+        <v>0.000238825690275333</v>
       </c>
     </row>
     <row r="265">
@@ -3082,7 +3082,7 @@
         </is>
       </c>
       <c r="B265" t="n">
-        <v>0.0002387108706652711</v>
+        <v>0.0002389429160665926</v>
       </c>
     </row>
     <row r="266">
@@ -3092,7 +3092,7 @@
         </is>
       </c>
       <c r="B266" t="n">
-        <v>0.0002374759229617852</v>
+        <v>0.000237698515910518</v>
       </c>
     </row>
     <row r="267">
@@ -3102,7 +3102,7 @@
         </is>
       </c>
       <c r="B267" t="n">
-        <v>0.000237206122063782</v>
+        <v>0.0002374200755896244</v>
       </c>
     </row>
     <row r="268">
@@ -3112,7 +3112,7 @@
         </is>
       </c>
       <c r="B268" t="n">
-        <v>0.0002366315849044821</v>
+        <v>0.0002368366182558548</v>
       </c>
     </row>
     <row r="269">
@@ -3122,7 +3122,7 @@
         </is>
       </c>
       <c r="B269" t="n">
-        <v>0.0002344161218567859</v>
+        <v>0.0002346114205157788</v>
       </c>
     </row>
     <row r="270">
@@ -3132,7 +3132,7 @@
         </is>
       </c>
       <c r="B270" t="n">
-        <v>0.0002374961368570782</v>
+        <v>0.000237685093166064</v>
       </c>
     </row>
     <row r="271">
@@ -3142,7 +3142,7 @@
         </is>
       </c>
       <c r="B271" t="n">
-        <v>0.0002336120522943796</v>
+        <v>0.0002337902793586009</v>
       </c>
     </row>
     <row r="272">
@@ -3152,7 +3152,7 @@
         </is>
       </c>
       <c r="B272" t="n">
-        <v>0.0002352066443327865</v>
+        <v>0.0002353774639172383</v>
       </c>
     </row>
     <row r="273">
@@ -3162,7 +3162,7 @@
         </is>
       </c>
       <c r="B273" t="n">
-        <v>0.000233505727621896</v>
+        <v>0.0002336675431887838</v>
       </c>
     </row>
     <row r="274">
@@ -3172,7 +3172,7 @@
         </is>
       </c>
       <c r="B274" t="n">
-        <v>0.0002315330526530316</v>
+        <v>0.0002316856620742784</v>
       </c>
     </row>
     <row r="275">
@@ -3182,7 +3182,7 @@
         </is>
       </c>
       <c r="B275" t="n">
-        <v>0.0002345045488734818</v>
+        <v>0.0002346504931495837</v>
       </c>
     </row>
     <row r="276">
@@ -3192,7 +3192,7 @@
         </is>
       </c>
       <c r="B276" t="n">
-        <v>0.0002309612199148796</v>
+        <v>0.0002310973442060711</v>
       </c>
     </row>
     <row r="277">
@@ -3202,7 +3202,7 @@
         </is>
       </c>
       <c r="B277" t="n">
-        <v>0.0002307234186539414</v>
+        <v>0.0002308515914892499</v>
       </c>
     </row>
     <row r="278">
@@ -3212,7 +3212,7 @@
         </is>
       </c>
       <c r="B278" t="n">
-        <v>0.0002322598438434339</v>
+        <v>0.000232380513094454</v>
       </c>
     </row>
     <row r="279">
@@ -3222,7 +3222,7 @@
         </is>
       </c>
       <c r="B279" t="n">
-        <v>0.0002296446258594729</v>
+        <v>0.0002297564125988278</v>
       </c>
     </row>
     <row r="280">
@@ -3232,7 +3232,7 @@
         </is>
       </c>
       <c r="B280" t="n">
-        <v>0.0002284664716655016</v>
+        <v>0.0002285700710537998</v>
       </c>
     </row>
     <row r="281">
@@ -3242,7 +3242,7 @@
         </is>
       </c>
       <c r="B281" t="n">
-        <v>0.0002309228549248638</v>
+        <v>0.0002310191579742968</v>
       </c>
     </row>
     <row r="282">
@@ -3252,7 +3252,7 @@
         </is>
       </c>
       <c r="B282" t="n">
-        <v>0.0002283278431554122</v>
+        <v>0.0002284156309239878</v>
       </c>
     </row>
     <row r="283">
@@ -3262,7 +3262,7 @@
         </is>
       </c>
       <c r="B283" t="n">
-        <v>0.0002271723355862423</v>
+        <v>0.0002272521659186875</v>
       </c>
     </row>
     <row r="284">
@@ -3272,7 +3272,7 @@
         </is>
       </c>
       <c r="B284" t="n">
-        <v>0.0002274223951025725</v>
+        <v>0.0002274944319760881</v>
       </c>
     </row>
     <row r="285">
@@ -3282,7 +3282,7 @@
         </is>
       </c>
       <c r="B285" t="n">
-        <v>0.0002278693762125571</v>
+        <v>0.0002279337526876858</v>
       </c>
     </row>
     <row r="286">
@@ -3292,7 +3292,7 @@
         </is>
       </c>
       <c r="B286" t="n">
-        <v>0.0002261610867352751</v>
+        <v>0.0002262176008389282</v>
       </c>
     </row>
     <row r="287">
@@ -3302,7 +3302,7 @@
         </is>
       </c>
       <c r="B287" t="n">
-        <v>0.0002249323830995375</v>
+        <v>0.0002249811166588656</v>
       </c>
     </row>
     <row r="288">
@@ -3312,7 +3312,7 @@
         </is>
       </c>
       <c r="B288" t="n">
-        <v>0.0002244273914172528</v>
+        <v>0.0002244686141733926</v>
       </c>
     </row>
     <row r="289">
@@ -3322,7 +3322,7 @@
         </is>
       </c>
       <c r="B289" t="n">
-        <v>0.0002261453805705376</v>
+        <v>0.0002261789412044727</v>
       </c>
     </row>
     <row r="290">
@@ -3332,7 +3332,7 @@
         </is>
       </c>
       <c r="B290" t="n">
-        <v>0.0002244329004188851</v>
+        <v>0.0002244589291390525</v>
       </c>
     </row>
     <row r="291">
@@ -3342,7 +3342,7 @@
         </is>
       </c>
       <c r="B291" t="n">
-        <v>0.0002234558991971926</v>
+        <v>0.0002234745005754906</v>
       </c>
     </row>
     <row r="292">
@@ -3352,7 +3352,7 @@
         </is>
       </c>
       <c r="B292" t="n">
-        <v>0.0002225620798024289</v>
+        <v>0.0002225732806446393</v>
       </c>
     </row>
     <row r="293">
@@ -3362,7 +3362,7 @@
         </is>
       </c>
       <c r="B293" t="n">
-        <v>0.0002219486366851246</v>
+        <v>0.000221952570790009</v>
       </c>
     </row>
     <row r="294">
@@ -3372,7 +3372,7 @@
         </is>
       </c>
       <c r="B294" t="n">
-        <v>0.0002213435024948566</v>
+        <v>0.0002213401262257863</v>
       </c>
     </row>
     <row r="295">
@@ -3382,7 +3382,7 @@
         </is>
       </c>
       <c r="B295" t="n">
-        <v>0.0002224012419481701</v>
+        <v>0.0002223902145910761</v>
       </c>
     </row>
     <row r="296">
@@ -3392,7 +3392,7 @@
         </is>
       </c>
       <c r="B296" t="n">
-        <v>0.000221572814117175</v>
+        <v>0.0002215546887671344</v>
       </c>
     </row>
     <row r="297">
@@ -3402,7 +3402,7 @@
         </is>
       </c>
       <c r="B297" t="n">
-        <v>0.0002206697895037515</v>
+        <v>0.0002206445895675662</v>
       </c>
     </row>
     <row r="298">
@@ -3412,7 +3412,7 @@
         </is>
       </c>
       <c r="B298" t="n">
-        <v>0.0002196408039179065</v>
+        <v>0.0002196085643831315</v>
       </c>
     </row>
     <row r="299">
@@ -3422,7 +3422,7 @@
         </is>
       </c>
       <c r="B299" t="n">
-        <v>0.0002193908919748004</v>
+        <v>0.0002193516076483762</v>
       </c>
     </row>
     <row r="300">
@@ -3432,7 +3432,7 @@
         </is>
       </c>
       <c r="B300" t="n">
-        <v>0.0002184664521322359</v>
+        <v>0.0002184202314329898</v>
       </c>
     </row>
     <row r="301">
@@ -3442,7 +3442,7 @@
         </is>
       </c>
       <c r="B301" t="n">
-        <v>0.0002180073000549977</v>
+        <v>0.0002179541577300397</v>
       </c>
     </row>
     <row r="302">
@@ -3452,7 +3452,7 @@
         </is>
       </c>
       <c r="B302" t="n">
-        <v>0.0002174991811015978</v>
+        <v>0.0002174391251228089</v>
       </c>
     </row>
     <row r="303">
@@ -3462,7 +3462,7 @@
         </is>
       </c>
       <c r="B303" t="n">
-        <v>0.0002171172691679483</v>
+        <v>0.0002170503518583569</v>
       </c>
     </row>
     <row r="304">
@@ -3472,7 +3472,7 @@
         </is>
       </c>
       <c r="B304" t="n">
-        <v>0.0002167097745726571</v>
+        <v>0.0002166360338959267</v>
       </c>
     </row>
     <row r="305">
@@ -3482,7 +3482,7 @@
         </is>
       </c>
       <c r="B305" t="n">
-        <v>0.0002162504100084734</v>
+        <v>0.0002161698927132517</v>
       </c>
     </row>
     <row r="306">
@@ -3492,7 +3492,7 @@
         </is>
       </c>
       <c r="B306" t="n">
-        <v>0.0002156055661521605</v>
+        <v>0.0002155183982714362</v>
       </c>
     </row>
     <row r="307">
@@ -3502,7 +3502,7 @@
         </is>
       </c>
       <c r="B307" t="n">
-        <v>0.0002151474238152324</v>
+        <v>0.0002150535539373201</v>
       </c>
     </row>
     <row r="308">
@@ -3512,7 +3512,7 @@
         </is>
       </c>
       <c r="B308" t="n">
-        <v>0.0002146858350531503</v>
+        <v>0.0002145853305914113</v>
       </c>
     </row>
     <row r="309">
@@ -3522,7 +3522,7 @@
         </is>
       </c>
       <c r="B309" t="n">
-        <v>0.0002141700326527738</v>
+        <v>0.0002140629757667044</v>
       </c>
     </row>
     <row r="310">
@@ -3532,7 +3532,7 @@
         </is>
       </c>
       <c r="B310" t="n">
-        <v>0.0002139161465580354</v>
+        <v>0.0002138024381971006</v>
       </c>
     </row>
     <row r="311">
@@ -3542,7 +3542,7 @@
         </is>
       </c>
       <c r="B311" t="n">
-        <v>0.0002132680953742204</v>
+        <v>0.0002131480045889696</v>
       </c>
     </row>
     <row r="312">
@@ -3552,7 +3552,7 @@
         </is>
       </c>
       <c r="B312" t="n">
-        <v>0.0002128323744685918</v>
+        <v>0.0002127057784465937</v>
       </c>
     </row>
     <row r="313">
@@ -3562,7 +3562,7 @@
         </is>
       </c>
       <c r="B313" t="n">
-        <v>0.0002123106192381889</v>
+        <v>0.0002121777113139273</v>
       </c>
     </row>
     <row r="314">
@@ -3572,7 +3572,7 @@
         </is>
       </c>
       <c r="B314" t="n">
-        <v>0.000211611007625013</v>
+        <v>0.0002114718722750808</v>
       </c>
     </row>
     <row r="315">
@@ -3582,7 +3582,7 @@
         </is>
       </c>
       <c r="B315" t="n">
-        <v>0.0002112721134792097</v>
+        <v>0.000211126626179151</v>
       </c>
     </row>
     <row r="316">
@@ -3592,7 +3592,7 @@
         </is>
       </c>
       <c r="B316" t="n">
-        <v>0.000210619945560179</v>
+        <v>0.0002104683460471664</v>
       </c>
     </row>
     <row r="317">
@@ -3602,7 +3602,7 @@
         </is>
       </c>
       <c r="B317" t="n">
-        <v>0.0002098878634637158</v>
+        <v>0.00020973029176351</v>
       </c>
     </row>
     <row r="318">
@@ -3612,7 +3612,7 @@
         </is>
       </c>
       <c r="B318" t="n">
-        <v>0.0002084864844932543</v>
+        <v>0.0002083237054410892</v>
       </c>
     </row>
     <row r="319">
@@ -3622,7 +3622,7 @@
         </is>
       </c>
       <c r="B319" t="n">
-        <v>0.000208973490298014</v>
+        <v>0.000208803706822165</v>
       </c>
     </row>
     <row r="320">
@@ -3632,7 +3632,7 @@
         </is>
       </c>
       <c r="B320" t="n">
-        <v>0.0002094567262999626</v>
+        <v>0.0002092799511514688</v>
       </c>
     </row>
     <row r="321">
@@ -3642,7 +3642,7 @@
         </is>
       </c>
       <c r="B321" t="n">
-        <v>0.0002085946183816587</v>
+        <v>0.0002084121014916438</v>
       </c>
     </row>
     <row r="322">
@@ -3652,7 +3652,7 @@
         </is>
       </c>
       <c r="B322" t="n">
-        <v>0.0002079902144615183</v>
+        <v>0.0002078018337301402</v>
       </c>
     </row>
     <row r="323">
@@ -3662,7 +3662,7 @@
         </is>
       </c>
       <c r="B323" t="n">
-        <v>0.0002073796172154967</v>
+        <v>0.0002071855300228839</v>
       </c>
     </row>
     <row r="324">
@@ -3672,7 +3672,7 @@
         </is>
       </c>
       <c r="B324" t="n">
-        <v>0.0002064015731444077</v>
+        <v>0.0002062021547310205</v>
       </c>
     </row>
     <row r="325">
@@ -3682,7 +3682,7 @@
         </is>
       </c>
       <c r="B325" t="n">
-        <v>0.0002047351223493145</v>
+        <v>0.0002045312591438069</v>
       </c>
     </row>
     <row r="326">
@@ -3692,7 +3692,7 @@
         </is>
       </c>
       <c r="B326" t="n">
-        <v>0.0002067831633620433</v>
+        <v>0.0002065706029828392</v>
       </c>
     </row>
     <row r="327">
@@ -3702,7 +3702,7 @@
         </is>
       </c>
       <c r="B327" t="n">
-        <v>0.000205994330123848</v>
+        <v>0.0002057762869745283</v>
       </c>
     </row>
     <row r="328">
@@ -3712,7 +3712,7 @@
         </is>
       </c>
       <c r="B328" t="n">
-        <v>0.0002053245135102443</v>
+        <v>0.0002051010843873629</v>
       </c>
     </row>
     <row r="329">
@@ -3722,7 +3722,7 @@
         </is>
       </c>
       <c r="B329" t="n">
-        <v>0.0002036826160080491</v>
+        <v>0.0002034549462696024</v>
       </c>
     </row>
     <row r="330">
@@ -3732,7 +3732,7 @@
         </is>
       </c>
       <c r="B330" t="n">
-        <v>0.0002028898547602805</v>
+        <v>0.0002026569850619881</v>
       </c>
     </row>
     <row r="331">
@@ -3742,7 +3742,7 @@
         </is>
       </c>
       <c r="B331" t="n">
-        <v>0.0002045101979561369</v>
+        <v>0.0002042690377348644</v>
       </c>
     </row>
     <row r="332">
@@ -3752,7 +3752,7 @@
         </is>
       </c>
       <c r="B332" t="n">
-        <v>0.0002034529400797076</v>
+        <v>0.0002032069315683828</v>
       </c>
     </row>
     <row r="333">
@@ -3762,7 +3762,7 @@
         </is>
       </c>
       <c r="B333" t="n">
-        <v>0.0002018509149013701</v>
+        <v>0.00020160103275584</v>
       </c>
     </row>
     <row r="334">
@@ -3772,7 +3772,7 @@
         </is>
       </c>
       <c r="B334" t="n">
-        <v>0.0002013965306591882</v>
+        <v>0.0002011412449795525</v>
       </c>
     </row>
     <row r="335">
@@ -3782,7 +3782,7 @@
         </is>
       </c>
       <c r="B335" t="n">
-        <v>0.0002025948978075284</v>
+        <v>0.0002023317853614295</v>
       </c>
     </row>
     <row r="336">
@@ -3792,7 +3792,7 @@
         </is>
       </c>
       <c r="B336" t="n">
-        <v>0.000201400210396112</v>
+        <v>0.0002011327041128395</v>
       </c>
     </row>
     <row r="337">
@@ -3802,7 +3802,7 @@
         </is>
       </c>
       <c r="B337" t="n">
-        <v>0.0001987824568830456</v>
+        <v>0.0001985129521463976</v>
       </c>
     </row>
     <row r="338">
@@ -3812,7 +3812,7 @@
         </is>
       </c>
       <c r="B338" t="n">
-        <v>0.0002014246163853034</v>
+        <v>0.0002011450145279645</v>
       </c>
     </row>
     <row r="339">
@@ -3822,7 +3822,7 @@
         </is>
       </c>
       <c r="B339" t="n">
-        <v>0.0002003023280990717</v>
+        <v>0.0002000184739520641</v>
       </c>
     </row>
     <row r="340">
@@ -3832,7 +3832,7 @@
         </is>
       </c>
       <c r="B340" t="n">
-        <v>0.0001970935174288183</v>
+        <v>0.0001968089370783468</v>
       </c>
     </row>
     <row r="341">
@@ -3842,7 +3842,7 @@
         </is>
       </c>
       <c r="B341" t="n">
-        <v>0.0002003796309917221</v>
+        <v>0.0002000837198291843</v>
       </c>
     </row>
     <row r="342">
@@ -3852,7 +3852,7 @@
         </is>
       </c>
       <c r="B342" t="n">
-        <v>0.0001991420503422885</v>
+        <v>0.0001988423134448363</v>
       </c>
     </row>
     <row r="343">
@@ -3862,7 +3862,7 @@
         </is>
       </c>
       <c r="B343" t="n">
-        <v>0.0001959102007271626</v>
+        <v>0.0001956100506054073</v>
       </c>
     </row>
     <row r="344">
@@ -3872,7 +3872,7 @@
         </is>
       </c>
       <c r="B344" t="n">
-        <v>0.0001990305485390841</v>
+        <v>0.0001987192186903312</v>
       </c>
     </row>
     <row r="345">
@@ -3882,7 +3882,7 @@
         </is>
       </c>
       <c r="B345" t="n">
-        <v>0.0001973437983896956</v>
+        <v>0.0001970295266118222</v>
       </c>
     </row>
     <row r="346">
@@ -3892,7 +3892,7 @@
         </is>
       </c>
       <c r="B346" t="n">
-        <v>0.0001953842553826968</v>
+        <v>0.0001950677608023729</v>
       </c>
     </row>
     <row r="347">
@@ -3902,7 +3902,7 @@
         </is>
       </c>
       <c r="B347" t="n">
-        <v>0.0001973377386472143</v>
+        <v>0.0001970118653781567</v>
       </c>
     </row>
     <row r="348">
@@ -3912,7 +3912,7 @@
         </is>
       </c>
       <c r="B348" t="n">
-        <v>0.0001947311747685378</v>
+        <v>0.0001944044206555783</v>
       </c>
     </row>
     <row r="349">
@@ -3922,7 +3922,7 @@
         </is>
       </c>
       <c r="B349" t="n">
-        <v>0.0001957988981274891</v>
+        <v>0.0001954644180020073</v>
       </c>
     </row>
     <row r="350">
@@ -3932,7 +3932,7 @@
         </is>
       </c>
       <c r="B350" t="n">
-        <v>0.0001952320097827477</v>
+        <v>0.0001948928737424399</v>
       </c>
     </row>
     <row r="351">
@@ -3942,7 +3942,7 @@
         </is>
       </c>
       <c r="B351" t="n">
-        <v>0.000193216211750361</v>
+        <v>0.0001928753306824013</v>
       </c>
     </row>
     <row r="352">
@@ -3952,7 +3952,7 @@
         </is>
       </c>
       <c r="B352" t="n">
-        <v>0.0001952142709985684</v>
+        <v>0.0001948638949156239</v>
       </c>
     </row>
     <row r="353">
@@ -3962,7 +3962,7 @@
         </is>
       </c>
       <c r="B353" t="n">
-        <v>0.000191884365233488</v>
+        <v>0.0001915350086290401</v>
       </c>
     </row>
     <row r="354">
@@ -3972,7 +3972,7 @@
         </is>
       </c>
       <c r="B354" t="n">
-        <v>0.0001947703057286603</v>
+        <v>0.0001944095442638796</v>
       </c>
     </row>
     <row r="355">
@@ -3982,7 +3982,7 @@
         </is>
       </c>
       <c r="B355" t="n">
-        <v>0.0001904793463391544</v>
+        <v>0.0001901217553412764</v>
       </c>
     </row>
     <row r="356">
@@ -3992,7 +3992,7 @@
         </is>
       </c>
       <c r="B356" t="n">
-        <v>0.0001942445426240163</v>
+        <v>0.0001938736740381181</v>
       </c>
     </row>
     <row r="357">
@@ -4002,7 +4002,7 @@
         </is>
       </c>
       <c r="B357" t="n">
-        <v>0.0001909422825015406</v>
+        <v>0.0001905727671069305</v>
       </c>
     </row>
     <row r="358">
@@ -4012,7 +4012,7 @@
         </is>
       </c>
       <c r="B358" t="n">
-        <v>0.0001920312299593347</v>
+        <v>0.000191653927901908</v>
       </c>
     </row>
     <row r="359">
@@ -4022,7 +4022,7 @@
         </is>
       </c>
       <c r="B359" t="n">
-        <v>0.0001904102603001775</v>
+        <v>0.0001900310167261299</v>
       </c>
     </row>
     <row r="360">
@@ -4032,7 +4032,7 @@
         </is>
       </c>
       <c r="B360" t="n">
-        <v>0.0001910469196474021</v>
+        <v>0.0001906608142842505</v>
       </c>
     </row>
     <row r="361">
@@ -4042,7 +4042,7 @@
         </is>
       </c>
       <c r="B361" t="n">
-        <v>0.0001894210164074375</v>
+        <v>0.0001890331761090656</v>
       </c>
     </row>
     <row r="362">
@@ -4052,7 +4052,7 @@
         </is>
       </c>
       <c r="B362" t="n">
-        <v>0.0001904587936553926</v>
+        <v>0.0001900632084120317</v>
       </c>
     </row>
     <row r="363">
@@ -4062,7 +4062,7 @@
         </is>
       </c>
       <c r="B363" t="n">
-        <v>0.0001872532471546188</v>
+        <v>0.0001868596090374098</v>
       </c>
     </row>
     <row r="364">
@@ -4072,7 +4072,7 @@
         </is>
       </c>
       <c r="B364" t="n">
-        <v>0.0001910283746448721</v>
+        <v>0.0001906206945222678</v>
       </c>
     </row>
     <row r="365">
@@ -4082,7 +4082,7 @@
         </is>
       </c>
       <c r="B365" t="n">
-        <v>0.0001866107262905769</v>
+        <v>0.0001862080397319376</v>
       </c>
     </row>
     <row r="366">
@@ -4092,7 +4092,7 @@
         </is>
       </c>
       <c r="B366" t="n">
-        <v>0.0001899539947462298</v>
+        <v>0.0001895381457658457</v>
       </c>
     </row>
     <row r="367">
@@ -4102,7 +4102,7 @@
         </is>
       </c>
       <c r="B367" t="n">
-        <v>0.0001861342475064581</v>
+        <v>0.0001857221364733371</v>
       </c>
     </row>
     <row r="368">
@@ -4112,7 +4112,7 @@
         </is>
       </c>
       <c r="B368" t="n">
-        <v>0.0001885815240339318</v>
+        <v>0.0001881584114615656</v>
       </c>
     </row>
     <row r="369">
@@ -4122,7 +4122,7 @@
         </is>
       </c>
       <c r="B369" t="n">
-        <v>0.0001861786530735957</v>
+        <v>0.0001857561303295855</v>
       </c>
     </row>
     <row r="370">
@@ -4132,7 +4132,7 @@
         </is>
       </c>
       <c r="B370" t="n">
-        <v>0.0001861154953280054</v>
+        <v>0.0001856879001005786</v>
       </c>
     </row>
     <row r="371">
@@ -4142,7 +4142,7 @@
         </is>
       </c>
       <c r="B371" t="n">
-        <v>0.0001866370272995013</v>
+        <v>0.0001862029663316842</v>
       </c>
     </row>
     <row r="372">
@@ -4152,7 +4152,7 @@
         </is>
       </c>
       <c r="B372" t="n">
-        <v>0.0001840937138005335</v>
+        <v>0.0001836609611662356</v>
       </c>
     </row>
     <row r="373">
@@ -4162,7 +4162,7 @@
         </is>
       </c>
       <c r="B373" t="n">
-        <v>0.0001866612010788513</v>
+        <v>0.0001862167472612492</v>
       </c>
     </row>
     <row r="374">
@@ -4172,7 +4172,7 @@
         </is>
       </c>
       <c r="B374" t="n">
-        <v>0.000184170978471865</v>
+        <v>0.0001837278472035103</v>
       </c>
     </row>
     <row r="375">
@@ -4182,7 +4182,7 @@
         </is>
       </c>
       <c r="B375" t="n">
-        <v>0.0001829178184528694</v>
+        <v>0.0001824729007408716</v>
       </c>
     </row>
     <row r="376">
@@ -4192,7 +4192,7 @@
         </is>
       </c>
       <c r="B376" t="n">
-        <v>0.0001859415886967101</v>
+        <v>0.00018548364258012</v>
       </c>
     </row>
     <row r="377">
@@ -4202,7 +4202,7 @@
         </is>
       </c>
       <c r="B377" t="n">
-        <v>0.0001825599776790877</v>
+        <v>0.0001821059938530235</v>
       </c>
     </row>
     <row r="378">
@@ -4212,7 +4212,7 @@
         </is>
       </c>
       <c r="B378" t="n">
-        <v>0.0001835137082889965</v>
+        <v>0.0001830521358906751</v>
       </c>
     </row>
     <row r="379">
@@ -4222,7 +4222,7 @@
         </is>
       </c>
       <c r="B379" t="n">
-        <v>0.0001830974495776136</v>
+        <v>0.0001826319423760933</v>
       </c>
     </row>
     <row r="380">
@@ -4232,7 +4232,7 @@
         </is>
       </c>
       <c r="B380" t="n">
-        <v>0.0001815358154292476</v>
+        <v>0.000181069751473052</v>
       </c>
     </row>
     <row r="381">
@@ -4242,7 +4242,7 @@
         </is>
       </c>
       <c r="B381" t="n">
-        <v>0.0001823833781491608</v>
+        <v>0.0001819099804948162</v>
       </c>
     </row>
     <row r="382">
@@ -4252,7 +4252,7 @@
         </is>
       </c>
       <c r="B382" t="n">
-        <v>0.0001820436862471298</v>
+        <v>0.0001815662736741846</v>
       </c>
     </row>
     <row r="383">
@@ -4262,7 +4262,7 @@
         </is>
       </c>
       <c r="B383" t="n">
-        <v>0.0001802473869726853</v>
+        <v>0.0001797701533740431</v>
       </c>
     </row>
     <row r="384">
@@ -4272,7 +4272,7 @@
         </is>
       </c>
       <c r="B384" t="n">
-        <v>0.0001801999633374295</v>
+        <v>0.0001797180372509651</v>
       </c>
     </row>
     <row r="385">
@@ -4282,7 +4282,7 @@
         </is>
       </c>
       <c r="B385" t="n">
-        <v>0.0001819319944504605</v>
+        <v>0.0001814402129842646</v>
       </c>
     </row>
     <row r="386">
@@ -4292,7 +4292,7 @@
         </is>
       </c>
       <c r="B386" t="n">
-        <v>0.0001795145289383416</v>
+        <v>0.0001790248907159208</v>
       </c>
     </row>
     <row r="387">
@@ -4302,7 +4302,7 @@
         </is>
       </c>
       <c r="B387" t="n">
-        <v>0.0001782331160010534</v>
+        <v>0.0001777423989599217</v>
       </c>
     </row>
     <row r="388">
@@ -4312,7 +4312,7 @@
         </is>
       </c>
       <c r="B388" t="n">
-        <v>0.0001807914850112297</v>
+        <v>0.0001802885160021907</v>
       </c>
     </row>
     <row r="389">
@@ -4322,7 +4322,7 @@
         </is>
       </c>
       <c r="B389" t="n">
-        <v>0.0001790755166015864</v>
+        <v>0.0001785728089335633</v>
       </c>
     </row>
     <row r="390">
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="B390" t="n">
-        <v>0.0001775237471999537</v>
+        <v>0.0001770208992995013</v>
       </c>
     </row>
     <row r="391">
@@ -4342,7 +4342,7 @@
         </is>
       </c>
       <c r="B391" t="n">
-        <v>0.0001769316003215932</v>
+        <v>0.0001764259352266419</v>
       </c>
     </row>
     <row r="392">
@@ -4352,7 +4352,7 @@
         </is>
       </c>
       <c r="B392" t="n">
-        <v>0.0001795265946557165</v>
+        <v>0.0001790082463175153</v>
       </c>
     </row>
     <row r="393">
@@ -4362,7 +4362,7 @@
         </is>
       </c>
       <c r="B393" t="n">
-        <v>0.0001774795030279841</v>
+        <v>0.0001769627679969986</v>
       </c>
     </row>
     <row r="394">
@@ -4372,7 +4372,7 @@
         </is>
       </c>
       <c r="B394" t="n">
-        <v>0.0001763798439404485</v>
+        <v>0.0001758618571053429</v>
       </c>
     </row>
     <row r="395">
@@ -4382,7 +4382,7 @@
         </is>
       </c>
       <c r="B395" t="n">
-        <v>0.0001754710020441865</v>
+        <v>0.0001749511975816546</v>
       </c>
     </row>
     <row r="396">
@@ -4392,7 +4392,7 @@
         </is>
       </c>
       <c r="B396" t="n">
-        <v>0.0001770138213866015</v>
+        <v>0.0001764845147029446</v>
       </c>
     </row>
     <row r="397">
@@ -4402,7 +4402,7 @@
         </is>
       </c>
       <c r="B397" t="n">
-        <v>0.000176501481449432</v>
+        <v>0.0001759692064447136</v>
       </c>
     </row>
     <row r="398">
@@ -4412,7 +4412,7 @@
         </is>
       </c>
       <c r="B398" t="n">
-        <v>0.0001752372863218153</v>
+        <v>0.0001747044798553577</v>
       </c>
     </row>
     <row r="399">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="B399" t="n">
-        <v>0.0001745111390660496</v>
+        <v>0.0001739761335833653</v>
       </c>
     </row>
     <row r="400">
@@ -4432,7 +4432,7 @@
         </is>
       </c>
       <c r="B400" t="n">
-        <v>0.0001737617770529767</v>
+        <v>0.000173224664050532</v>
       </c>
     </row>
     <row r="401">
@@ -4442,7 +4442,7 @@
         </is>
       </c>
       <c r="B401" t="n">
-        <v>0.0001748665094502518</v>
+        <v>0.0001743213147918089</v>
       </c>
     </row>
     <row r="402">
@@ -4452,7 +4452,7 @@
         </is>
       </c>
       <c r="B402" t="n">
-        <v>0.0001750326881077918</v>
+        <v>0.0001744823699002688</v>
       </c>
     </row>
     <row r="403">
@@ -4462,7 +4462,7 @@
         </is>
       </c>
       <c r="B403" t="n">
-        <v>0.0001734751342853456</v>
+        <v>0.000172925423047331</v>
       </c>
     </row>
     <row r="404">
@@ -4472,7 +4472,7 @@
         </is>
       </c>
       <c r="B404" t="n">
-        <v>0.0001731161457791652</v>
+        <v>0.0001725633111895334</v>
       </c>
     </row>
     <row r="405">
@@ -4482,7 +4482,7 @@
         </is>
       </c>
       <c r="B405" t="n">
-        <v>0.0001721849036246717</v>
+        <v>0.000171630646619734</v>
       </c>
     </row>
     <row r="406">
@@ -4492,7 +4492,7 @@
         </is>
       </c>
       <c r="B406" t="n">
-        <v>0.0001720116796005922</v>
+        <v>0.0001714537623759227</v>
       </c>
     </row>
     <row r="407">
@@ -4502,7 +4502,7 @@
         </is>
       </c>
       <c r="B407" t="n">
-        <v>0.0001713994573106755</v>
+        <v>0.0001708391696444342</v>
       </c>
     </row>
     <row r="408">
@@ -4512,7 +4512,7 @@
         </is>
       </c>
       <c r="B408" t="n">
-        <v>0.00017320802302131</v>
+        <v>0.0001726370882568332</v>
       </c>
     </row>
     <row r="409">
@@ -4522,7 +4522,7 @@
         </is>
       </c>
       <c r="B409" t="n">
-        <v>0.0001716465735060923</v>
+        <v>0.0001710766060371847</v>
       </c>
     </row>
     <row r="410">
@@ -4532,7 +4532,7 @@
         </is>
       </c>
       <c r="B410" t="n">
-        <v>0.0001712905936028812</v>
+        <v>0.0001707175824555889</v>
       </c>
     </row>
     <row r="411">
@@ -4542,7 +4542,7 @@
         </is>
       </c>
       <c r="B411" t="n">
-        <v>0.0001706144423077969</v>
+        <v>0.0001700395074902476</v>
       </c>
     </row>
     <row r="412">
@@ -4552,7 +4552,7 @@
         </is>
       </c>
       <c r="B412" t="n">
-        <v>0.0001700235864627925</v>
+        <v>0.0001694463914653777</v>
       </c>
     </row>
     <row r="413">
@@ -4562,7 +4562,7 @@
         </is>
       </c>
       <c r="B413" t="n">
-        <v>0.000169615663608928</v>
+        <v>0.0001690356759728534</v>
       </c>
     </row>
     <row r="414">
@@ -4572,7 +4572,7 @@
         </is>
       </c>
       <c r="B414" t="n">
-        <v>0.0001693975605636201</v>
+        <v>0.0001688141162935747</v>
       </c>
     </row>
     <row r="415">
@@ -4582,7 +4582,7 @@
         </is>
       </c>
       <c r="B415" t="n">
-        <v>0.0001688563759134431</v>
+        <v>0.0001682706485724538</v>
       </c>
     </row>
     <row r="416">
@@ -4592,7 +4592,7 @@
         </is>
       </c>
       <c r="B416" t="n">
-        <v>0.000168610162585087</v>
+        <v>0.0001680211275244044</v>
       </c>
     </row>
     <row r="417">
@@ -4602,7 +4602,7 @@
         </is>
       </c>
       <c r="B417" t="n">
-        <v>0.0001681286022008787</v>
+        <v>0.0001675370616642533</v>
       </c>
     </row>
     <row r="418">
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="B418" t="n">
-        <v>0.0001678510889051409</v>
+        <v>0.0001672564528929939</v>
       </c>
     </row>
     <row r="419">
@@ -4622,7 +4622,7 @@
         </is>
       </c>
       <c r="B419" t="n">
-        <v>0.0001690412463317454</v>
+        <v>0.0001684379427605901</v>
       </c>
     </row>
     <row r="420">
@@ -4632,7 +4632,7 @@
         </is>
       </c>
       <c r="B420" t="n">
-        <v>0.0001679059368656466</v>
+        <v>0.0001673026587561894</v>
       </c>
     </row>
     <row r="421">
@@ -4642,7 +4642,7 @@
         </is>
       </c>
       <c r="B421" t="n">
-        <v>0.0001674400677549148</v>
+        <v>0.0001668344319156798</v>
       </c>
     </row>
     <row r="422">
@@ -4652,7 +4652,7 @@
         </is>
       </c>
       <c r="B422" t="n">
-        <v>0.000166924852096241</v>
+        <v>0.0001663170112265206</v>
       </c>
     </row>
     <row r="423">
@@ -4662,7 +4662,7 @@
         </is>
       </c>
       <c r="B423" t="n">
-        <v>0.0001665155560685777</v>
+        <v>0.0001659051808035534</v>
       </c>
     </row>
     <row r="424">
@@ -4672,7 +4672,7 @@
         </is>
       </c>
       <c r="B424" t="n">
-        <v>0.0001661871338057518</v>
+        <v>0.0001655739343163285</v>
       </c>
     </row>
     <row r="425">
@@ -4682,7 +4682,7 @@
         </is>
       </c>
       <c r="B425" t="n">
-        <v>0.0001658324376796658</v>
+        <v>0.0001652165232624138</v>
       </c>
     </row>
     <row r="426">
@@ -4692,7 +4692,7 @@
         </is>
       </c>
       <c r="B426" t="n">
-        <v>0.0001655041429172844</v>
+        <v>0.0001648854458459254</v>
       </c>
     </row>
     <row r="427">
@@ -4702,7 +4702,7 @@
         </is>
       </c>
       <c r="B427" t="n">
-        <v>0.0001649876015678553</v>
+        <v>0.0001643668738130355</v>
       </c>
     </row>
     <row r="428">
@@ -4712,7 +4712,7 @@
         </is>
       </c>
       <c r="B428" t="n">
-        <v>0.0001647924007763967</v>
+        <v>0.0001641684356052508</v>
       </c>
     </row>
     <row r="429">
@@ -4722,7 +4722,7 @@
         </is>
       </c>
       <c r="B429" t="n">
-        <v>0.0001643556442114255</v>
+        <v>0.0001637294005541765</v>
       </c>
     </row>
     <row r="430">
@@ -4732,7 +4732,7 @@
         </is>
       </c>
       <c r="B430" t="n">
-        <v>0.0001639768222913634</v>
+        <v>0.0001633480410106834</v>
       </c>
     </row>
     <row r="431">
@@ -4742,7 +4742,7 @@
         </is>
       </c>
       <c r="B431" t="n">
-        <v>0.0001635885926846334</v>
+        <v>0.0001629574696710091</v>
       </c>
     </row>
     <row r="432">
@@ -4752,7 +4752,7 @@
         </is>
       </c>
       <c r="B432" t="n">
-        <v>0.0001634463231668221</v>
+        <v>0.0001628118430737205</v>
       </c>
     </row>
     <row r="433">
@@ -4762,7 +4762,7 @@
         </is>
       </c>
       <c r="B433" t="n">
-        <v>0.0001627396755418653</v>
+        <v>0.0001621041040781475</v>
       </c>
     </row>
     <row r="434">
@@ -4772,7 +4772,7 @@
         </is>
       </c>
       <c r="B434" t="n">
-        <v>0.0001623002722187583</v>
+        <v>0.0001616625998841203</v>
       </c>
     </row>
     <row r="435">
@@ -4782,7 +4782,7 @@
         </is>
       </c>
       <c r="B435" t="n">
-        <v>0.0001609696942104115</v>
+        <v>0.0001603336050603596</v>
       </c>
     </row>
     <row r="436">
@@ -4792,7 +4792,7 @@
         </is>
       </c>
       <c r="B436" t="n">
-        <v>0.0001623743731207274</v>
+        <v>0.000161728576438161</v>
       </c>
     </row>
     <row r="437">
@@ -4802,7 +4802,7 @@
         </is>
       </c>
       <c r="B437" t="n">
-        <v>0.0001622523178961393</v>
+        <v>0.0001616032362388309</v>
       </c>
     </row>
     <row r="438">
@@ -4812,7 +4812,7 @@
         </is>
       </c>
       <c r="B438" t="n">
-        <v>0.0001616068570915524</v>
+        <v>0.0001609564613091036</v>
       </c>
     </row>
     <row r="439">
@@ -4822,7 +4822,7 @@
         </is>
       </c>
       <c r="B439" t="n">
-        <v>0.0001615900826421427</v>
+        <v>0.000160936035340264</v>
       </c>
     </row>
     <row r="440">
@@ -4832,7 +4832,7 @@
         </is>
       </c>
       <c r="B440" t="n">
-        <v>0.0001609674459896264</v>
+        <v>0.00016031209540496</v>
       </c>
     </row>
     <row r="441">
@@ -4842,7 +4842,7 @@
         </is>
       </c>
       <c r="B441" t="n">
-        <v>0.0001607680885982726</v>
+        <v>0.000160109799957808</v>
       </c>
     </row>
     <row r="442">
@@ -4852,7 +4852,7 @@
         </is>
       </c>
       <c r="B442" t="n">
-        <v>0.0001321045309465679</v>
+        <v>0.0001315657209878675</v>
       </c>
     </row>
     <row r="443">
@@ -4862,7 +4862,7 @@
         </is>
       </c>
       <c r="B443" t="n">
-        <v>0.0001099601766063979</v>
+        <v>0.0001095133306798814</v>
       </c>
     </row>
     <row r="444">
@@ -4872,7 +4872,7 @@
         </is>
       </c>
       <c r="B444" t="n">
-        <v>9.545411287692287e-05</v>
+        <v>9.506679880922452e-05</v>
       </c>
     </row>
     <row r="445">
@@ -4882,7 +4882,7 @@
         </is>
       </c>
       <c r="B445" t="n">
-        <v>8.33617713058822e-05</v>
+        <v>8.302372239677334e-05</v>
       </c>
     </row>
     <row r="446">
@@ -4892,7 +4892,7 @@
         </is>
       </c>
       <c r="B446" t="n">
-        <v>7.33591457911445e-05</v>
+        <v>7.306170410846653e-05</v>
       </c>
     </row>
     <row r="447">
@@ -4902,7 +4902,7 @@
         </is>
       </c>
       <c r="B447" t="n">
-        <v>6.41882008541113e-05</v>
+        <v>6.392789792695485e-05</v>
       </c>
     </row>
     <row r="448">
@@ -4912,7 +4912,7 @@
         </is>
       </c>
       <c r="B448" t="n">
-        <v>5.600042816401024e-05</v>
+        <v>5.577323057519902e-05</v>
       </c>
     </row>
     <row r="449">
@@ -4922,7 +4922,7 @@
         </is>
       </c>
       <c r="B449" t="n">
-        <v>4.823620772426093e-05</v>
+        <v>4.804036304370082e-05</v>
       </c>
     </row>
     <row r="450">
@@ -4932,7 +4932,7 @@
         </is>
       </c>
       <c r="B450" t="n">
-        <v>4.112611406623008e-05</v>
+        <v>4.095899030777348e-05</v>
       </c>
     </row>
     <row r="451">
@@ -4942,7 +4942,7 @@
         </is>
       </c>
       <c r="B451" t="n">
-        <v>3.456493349042162e-05</v>
+        <v>3.442429712889341e-05</v>
       </c>
     </row>
     <row r="452">
@@ -4952,7 +4952,7 @@
         </is>
       </c>
       <c r="B452" t="n">
-        <v>2.812650615045032e-05</v>
+        <v>2.801190312478432e-05</v>
       </c>
     </row>
     <row r="453">
@@ -4962,7 +4962,7 @@
         </is>
       </c>
       <c r="B453" t="n">
-        <v>2.209936294135911e-05</v>
+        <v>2.200914208970507e-05</v>
       </c>
     </row>
     <row r="454">
@@ -4972,7 +4972,7 @@
         </is>
       </c>
       <c r="B454" t="n">
-        <v>1.752072275827146e-05</v>
+        <v>1.744906044821517e-05</v>
       </c>
     </row>
     <row r="455">
@@ -4982,7 +4982,7 @@
         </is>
       </c>
       <c r="B455" t="n">
-        <v>1.471870772680193e-05</v>
+        <v>1.465843596515558e-05</v>
       </c>
     </row>
     <row r="456">
@@ -4992,7 +4992,7 @@
         </is>
       </c>
       <c r="B456" t="n">
-        <v>1.208083030354781e-05</v>
+        <v>1.203130039682682e-05</v>
       </c>
     </row>
     <row r="457">
@@ -5002,7 +5002,7 @@
         </is>
       </c>
       <c r="B457" t="n">
-        <v>9.553885261444565e-06</v>
+        <v>9.514667722979387e-06</v>
       </c>
     </row>
     <row r="458">
@@ -5012,7 +5012,7 @@
         </is>
       </c>
       <c r="B458" t="n">
-        <v>7.137414364739505e-06</v>
+        <v>7.108080664709841e-06</v>
       </c>
     </row>
     <row r="459">
@@ -5022,7 +5022,7 @@
         </is>
       </c>
       <c r="B459" t="n">
-        <v>4.752939562306036e-06</v>
+        <v>4.73337947076055e-06</v>
       </c>
     </row>
     <row r="460">
@@ -5032,7 +5032,7 @@
         </is>
       </c>
       <c r="B460" t="n">
-        <v>2.478196196667812e-06</v>
+        <v>2.467984501739037e-06</v>
       </c>
     </row>
     <row r="461">
@@ -5042,7 +5042,7 @@
         </is>
       </c>
       <c r="B461" t="n">
-        <v>4.169883380079651e-07</v>
+        <v>4.152686817186842e-07</v>
       </c>
     </row>
     <row r="462">

</xml_diff>